<commit_message>
Correction In Import Data
</commit_message>
<xml_diff>
--- a/HRMS.UI/wwwroot/SampleTemplates/MonthlyDeductionTemplate1.xlsx
+++ b/HRMS.UI/wwwroot/SampleTemplates/MonthlyDeductionTemplate1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Alpha_Emp_code</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>GroupMedical</t>
+  </si>
+  <si>
+    <t>Loan</t>
   </si>
 </sst>
 </file>
@@ -104,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -113,6 +116,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -404,7 +408,7 @@
     <col min="1" max="1" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -435,8 +439,11 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>10678</v>
       </c>
@@ -467,8 +474,11 @@
       <c r="J2" s="2">
         <v>800</v>
       </c>
+      <c r="K2" s="2">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>10679</v>
       </c>
@@ -498,9 +508,13 @@
       </c>
       <c r="J3" s="2">
         <v>750</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>